<commit_message>
Show route as graph
</commit_message>
<xml_diff>
--- a/stations_data.xlsx
+++ b/stations_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holog\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holog\Desktop\route_finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C7FCDD-4BD3-4E14-B713-ADAD4017DD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184BB2D0-9726-4CFA-BD38-A29556121465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E27EB14-FE98-48A4-8B37-E50CC61CB50C}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -611,50 +611,80 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
+      <c r="C14">
+        <v>36.299999999999997</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>5</v>
       </c>
+      <c r="C15">
+        <v>13.2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
+      </c>
+      <c r="C22">
+        <v>38.299999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full stations excel data
</commit_message>
<xml_diff>
--- a/stations_data.xlsx
+++ b/stations_data.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holog\Desktop\route_finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD545BD-CCD5-4C2F-9EA4-C3AC36EFEF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4240C01-2850-4466-B2AB-0F8FCBE267C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E27EB14-FE98-48A4-8B37-E50CC61CB50C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$364</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">Sheet1!$B$1:$B$364</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$E:$E</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="302">
   <si>
     <t>Line</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -494,10 +499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HQU1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -691,6 +692,562 @@
   </si>
   <si>
     <t>CXP12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Station_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Station_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree (Nether)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sky city (Lower)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creeper farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train testing station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sky city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Large piston elevator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shulker box loaders</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sea edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vacantcraft builds sea edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mini elevator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color world</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue EXPRESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Purple line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pink line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train testing station line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Underground passageway</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Treehouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train bridge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train branch test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train leaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample donut circle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>South sea interchange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample request stop and express line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample same direction short station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample long station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single double loop unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample different direction short station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample branch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train testing station sea edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eagle station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stone generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Holo's house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rocket / UFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modern station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Industrial station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double item vending machine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wall item swap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RNG Machine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ground item swap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hidden base garden</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elevator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass (Donut circle)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Viewing point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instant shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bidrectional train station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quartz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Air resort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water elevator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potion farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Block item swap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass south</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water bridge door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Piston sea edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note block</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Village shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Piston central</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stack item shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sky tower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>North donut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main (Lower level)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>South donut underground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Piston extender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regenerative wall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sky tower (Second floor)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lava and water dispensers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drumstick top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inside cake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diamond trap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concrete launcher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enormous elevator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4x4 Piston door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2x4 Piston door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water dispenser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oak tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single item extractor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lever to button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2x2 Hole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4x4 Door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beacon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spawner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quartz bridge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bamboo farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Love shrine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Holo's heritage station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Custom doors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hidden basement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drumstick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass (Sealine)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sky city (Sakura garden)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soul sand guardian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Planet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glass platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>West coral</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guardian farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>South coral</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enderman killer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slime launcher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mass item dispenser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMP Terminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dark oak tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raid farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raid drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minecart mob farm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>South sea explorer line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut circle (Brown)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut circle (Light gray)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut circle (Gray)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut circle (Lime)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut circle (Orange)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Highspeed (Sky city &lt;&gt; TTS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Highspeed (Donut &lt;&gt; Modern)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donut underground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heritage sky tower line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heritage loop line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heritage quartz line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sealine surfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral express (West coral express)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral express (Guardian farm shuttle)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral express (South coral express)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral express (Enderman killer express)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coral express main line</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1084,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722DD655-737C-4A3A-ADF0-EF575C5049FC}">
-  <dimension ref="A1:C364"/>
+  <dimension ref="A1:I364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
-      <selection activeCell="C365" sqref="C365"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1096,9 +1653,13 @@
     <col min="2" max="2" width="24.75" customWidth="1"/>
     <col min="3" max="3" width="25.625" customWidth="1"/>
     <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="36.75" customWidth="1"/>
+    <col min="8" max="8" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="40.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,8 +1669,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1119,80 +1692,214 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
         <v>48.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
         <v>17.399999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7">
         <v>58.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
         <v>48.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11">
         <v>52.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1202,80 +1909,214 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14">
         <v>36.299999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19">
         <v>40.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>188</v>
+      </c>
+      <c r="H19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>189</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>190</v>
+      </c>
+      <c r="H21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22">
         <v>38.299999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>191</v>
+      </c>
+      <c r="H22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1285,40 +2126,114 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25">
         <v>31.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>194</v>
+      </c>
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>19</v>
       </c>
       <c r="C26">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>195</v>
+      </c>
+      <c r="H26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>196</v>
+      </c>
+      <c r="H27" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28">
         <v>36.200000000000003</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1328,48 +2243,134 @@
       <c r="C30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31">
         <v>31.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>202</v>
+      </c>
+      <c r="H31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>19</v>
       </c>
       <c r="C32">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" t="s">
+        <v>201</v>
+      </c>
+      <c r="H32" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>20</v>
       </c>
       <c r="C33">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>204</v>
+      </c>
+      <c r="H33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="C34">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>203</v>
+      </c>
+      <c r="H35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>205</v>
+      </c>
+      <c r="H36" t="s">
+        <v>130</v>
+      </c>
+      <c r="I36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1379,80 +2380,228 @@
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" t="s">
+        <v>134</v>
+      </c>
+      <c r="I37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" t="s">
+        <v>207</v>
+      </c>
+      <c r="H38" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>24</v>
       </c>
       <c r="C39">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>25</v>
       </c>
       <c r="C40">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" t="s">
+        <v>281</v>
+      </c>
+      <c r="I40" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" t="s">
+        <v>210</v>
+      </c>
+      <c r="H41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I41" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>26</v>
       </c>
       <c r="C42">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
+        <v>211</v>
+      </c>
+      <c r="H42" t="s">
+        <v>142</v>
+      </c>
+      <c r="I42" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>10</v>
       </c>
       <c r="C43">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" t="s">
+        <v>212</v>
+      </c>
+      <c r="H43" t="s">
+        <v>144</v>
+      </c>
+      <c r="I43" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>27</v>
       </c>
       <c r="C44">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="s">
+        <v>213</v>
+      </c>
+      <c r="H44" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>28</v>
       </c>
       <c r="C45">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" t="s">
+        <v>214</v>
+      </c>
+      <c r="H45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" t="s">
+        <v>215</v>
+      </c>
+      <c r="H46" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" t="s">
+        <v>216</v>
+      </c>
+      <c r="H47" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" t="s">
+        <v>217</v>
+      </c>
+      <c r="H48" t="s">
+        <v>159</v>
+      </c>
+      <c r="I48" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -1462,96 +2611,200 @@
       <c r="C49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" t="s">
+        <v>218</v>
+      </c>
+      <c r="H49" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>23</v>
       </c>
       <c r="C50">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" t="s">
+        <v>219</v>
+      </c>
+      <c r="H50" t="s">
+        <v>160</v>
+      </c>
+      <c r="I50" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>24</v>
       </c>
       <c r="C51">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" t="s">
+        <v>220</v>
+      </c>
+      <c r="H51" t="s">
+        <v>161</v>
+      </c>
+      <c r="I51" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>25</v>
       </c>
       <c r="C52">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" t="s">
+        <v>221</v>
+      </c>
+      <c r="H52" t="s">
+        <v>162</v>
+      </c>
+      <c r="I52" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>14</v>
       </c>
       <c r="C53">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>26</v>
       </c>
       <c r="C54">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>10</v>
       </c>
       <c r="C55">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>31</v>
       </c>
       <c r="C56">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>32</v>
       </c>
       <c r="C57">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>33</v>
       </c>
       <c r="C58">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>34</v>
       </c>
       <c r="C59">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>76</v>
+      </c>
+      <c r="F59" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>29</v>
       </c>
       <c r="C60">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -1561,88 +2814,162 @@
       <c r="C62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F62" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>23</v>
       </c>
       <c r="C63">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>24</v>
       </c>
       <c r="C64">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>25</v>
       </c>
       <c r="C65">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>14</v>
       </c>
       <c r="C66">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>26</v>
       </c>
       <c r="C67">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>94</v>
+      </c>
+      <c r="F67" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="C68">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E68" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>31</v>
       </c>
       <c r="C69">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E69" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>32</v>
       </c>
       <c r="C70">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>99</v>
+      </c>
+      <c r="F70" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>36</v>
       </c>
       <c r="C71">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E71" t="s">
+        <v>100</v>
+      </c>
+      <c r="F71" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>37</v>
       </c>
       <c r="C72">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>102</v>
+      </c>
+      <c r="F72" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E73" t="s">
+        <v>103</v>
+      </c>
+      <c r="F73" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -1652,16 +2979,36 @@
       <c r="C74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E74" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>39</v>
       </c>
       <c r="C75">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E75" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E76" t="s">
+        <v>106</v>
+      </c>
+      <c r="F76" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>40</v>
       </c>
@@ -1671,56 +3018,106 @@
       <c r="C77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E77" t="s">
+        <v>107</v>
+      </c>
+      <c r="F77" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>41</v>
       </c>
       <c r="C78">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E78" t="s">
+        <v>108</v>
+      </c>
+      <c r="F78" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>42</v>
       </c>
       <c r="C79">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E79" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>20</v>
       </c>
       <c r="C80">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>16</v>
       </c>
       <c r="C81">
         <v>22.9</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E81" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>43</v>
       </c>
       <c r="C82">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>112</v>
+      </c>
+      <c r="F82" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>44</v>
       </c>
       <c r="C83">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E83" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E84" t="s">
+        <v>115</v>
+      </c>
+      <c r="F84" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -1730,40 +3127,78 @@
       <c r="C85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E85" t="s">
+        <v>116</v>
+      </c>
+      <c r="F85" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>46</v>
       </c>
       <c r="C86">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>117</v>
+      </c>
+      <c r="F86" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>29</v>
       </c>
       <c r="C87">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>118</v>
+      </c>
+      <c r="F87" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>47</v>
       </c>
       <c r="C88">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E88" t="s">
+        <v>120</v>
+      </c>
+      <c r="F88" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>44</v>
       </c>
       <c r="C89">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E89" t="s">
+        <v>121</v>
+      </c>
+      <c r="F89" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E90" t="s">
+        <v>122</v>
+      </c>
+      <c r="F90" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -1773,32 +3208,64 @@
       <c r="C91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E91" t="s">
+        <v>124</v>
+      </c>
+      <c r="F91" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>46</v>
       </c>
       <c r="C92">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E92" t="s">
+        <v>125</v>
+      </c>
+      <c r="F92" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>29</v>
       </c>
       <c r="C93">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E93" t="s">
+        <v>127</v>
+      </c>
+      <c r="F93" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>49</v>
       </c>
       <c r="C94">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E94" t="s">
+        <v>128</v>
+      </c>
+      <c r="F94" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E95" t="s">
+        <v>131</v>
+      </c>
+      <c r="F95" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>50</v>
       </c>
@@ -1808,96 +3275,176 @@
       <c r="C96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E96" t="s">
+        <v>132</v>
+      </c>
+      <c r="F96" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>14</v>
       </c>
       <c r="C97">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E97" t="s">
+        <v>133</v>
+      </c>
+      <c r="F97" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>51</v>
       </c>
       <c r="C98">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E98" t="s">
+        <v>135</v>
+      </c>
+      <c r="F98" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>42</v>
       </c>
       <c r="C99">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E99" t="s">
+        <v>137</v>
+      </c>
+      <c r="F99" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>52</v>
       </c>
       <c r="C100">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E100" t="s">
+        <v>139</v>
+      </c>
+      <c r="F100" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>53</v>
       </c>
       <c r="C101">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E101" t="s">
+        <v>141</v>
+      </c>
+      <c r="F101" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>68</v>
       </c>
       <c r="C102">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E102" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>54</v>
       </c>
       <c r="C103">
         <v>7</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E103" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>6</v>
       </c>
       <c r="C104">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E104" t="s">
+        <v>147</v>
+      </c>
+      <c r="F104" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>55</v>
       </c>
       <c r="C105">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E105" t="s">
+        <v>149</v>
+      </c>
+      <c r="F105" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>56</v>
       </c>
       <c r="C106">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E106" t="s">
+        <v>150</v>
+      </c>
+      <c r="F106" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>57</v>
       </c>
       <c r="C107">
         <v>13.1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E107" t="s">
+        <v>152</v>
+      </c>
+      <c r="F107" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E108" t="s">
+        <v>154</v>
+      </c>
+      <c r="F108" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>58</v>
       </c>
@@ -1907,24 +3454,42 @@
       <c r="C109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F109" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>59</v>
       </c>
       <c r="C110">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E110" t="s">
+        <v>156</v>
+      </c>
+      <c r="F110" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>60</v>
       </c>
       <c r="C111">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E111" t="s">
+        <v>157</v>
+      </c>
+      <c r="F111" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>20</v>
       </c>
@@ -2686,7 +4251,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B217" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="C217">
         <v>10.1</v>
@@ -2702,10 +4267,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
+        <v>114</v>
+      </c>
+      <c r="B220" t="s">
         <v>115</v>
-      </c>
-      <c r="B220" t="s">
-        <v>116</v>
       </c>
       <c r="C220">
         <v>0</v>
@@ -2713,7 +4278,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B221" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C221">
         <v>7.1</v>
@@ -2721,7 +4286,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C222">
         <v>10.6</v>
@@ -2729,7 +4294,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B223" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C223">
         <v>5.7</v>
@@ -2753,10 +4318,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B227" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C227">
         <v>0</v>
@@ -2764,7 +4329,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B228" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C228">
         <v>7.1</v>
@@ -2772,7 +4337,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C229">
         <v>10.6</v>
@@ -2780,7 +4345,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C230">
         <v>5.7</v>
@@ -2796,7 +4361,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B232" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C232">
         <v>11.1</v>
@@ -2804,7 +4369,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B233" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C233">
         <v>6.3</v>
@@ -2812,7 +4377,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B234" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C234">
         <v>8</v>
@@ -2828,10 +4393,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
+        <v>123</v>
+      </c>
+      <c r="B237" t="s">
         <v>124</v>
-      </c>
-      <c r="B237" t="s">
-        <v>125</v>
       </c>
       <c r="C237">
         <v>0</v>
@@ -2839,7 +4404,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B238" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C238">
         <v>7</v>
@@ -2847,7 +4412,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B239" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C239">
         <v>6.6</v>
@@ -2855,7 +4420,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B240" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C240">
         <v>14.5</v>
@@ -2863,7 +4428,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C241">
         <v>6.3</v>
@@ -2871,7 +4436,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B242" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C242">
         <v>8</v>
@@ -2887,7 +4452,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B245" t="s">
         <v>4</v>
@@ -2922,7 +4487,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B249" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C249">
         <v>18.5</v>
@@ -2938,7 +4503,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B251" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C251">
         <v>35.700000000000003</v>
@@ -2954,7 +4519,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B254" t="s">
         <v>83</v>
@@ -2965,7 +4530,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B255" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C255">
         <v>12</v>
@@ -2981,7 +4546,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B257" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C257">
         <v>35.700000000000003</v>
@@ -2997,10 +4562,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
+        <v>130</v>
+      </c>
+      <c r="B260" t="s">
         <v>131</v>
-      </c>
-      <c r="B260" t="s">
-        <v>132</v>
       </c>
       <c r="C260">
         <v>0</v>
@@ -3016,7 +4581,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B262" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C262">
         <v>24</v>
@@ -3024,7 +4589,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B263" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C263">
         <v>19.8</v>
@@ -3032,7 +4597,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B264" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C264">
         <v>7</v>
@@ -3040,7 +4605,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B265" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C265">
         <v>15</v>
@@ -3048,7 +4613,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B266" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C266">
         <v>23.7</v>
@@ -3056,7 +4621,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B267" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C267">
         <v>17.8</v>
@@ -3072,10 +4637,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B270" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C270">
         <v>0</v>
@@ -3091,7 +4656,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B272" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C272">
         <v>24</v>
@@ -3099,7 +4664,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B273" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C273">
         <v>19.8</v>
@@ -3107,7 +4672,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B274" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C274">
         <v>7</v>
@@ -3115,7 +4680,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B275" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C275">
         <v>15</v>
@@ -3123,7 +4688,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B276" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C276">
         <v>16.7</v>
@@ -3131,10 +4696,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
+        <v>136</v>
+      </c>
+      <c r="B278" t="s">
         <v>137</v>
-      </c>
-      <c r="B278" t="s">
-        <v>138</v>
       </c>
       <c r="C278">
         <v>0</v>
@@ -3142,7 +4707,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B279" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C279">
         <v>9.4</v>
@@ -3166,7 +4731,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B282" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C282">
         <v>8.1</v>
@@ -3174,10 +4739,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
+        <v>138</v>
+      </c>
+      <c r="B284" t="s">
         <v>139</v>
-      </c>
-      <c r="B284" t="s">
-        <v>140</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -3193,10 +4758,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
+        <v>140</v>
+      </c>
+      <c r="B287" t="s">
         <v>141</v>
-      </c>
-      <c r="B287" t="s">
-        <v>142</v>
       </c>
       <c r="C287">
         <v>0</v>
@@ -3212,7 +4777,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B290" t="s">
         <v>12</v>
@@ -3223,7 +4788,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B291" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C291">
         <v>18.3</v>
@@ -3231,7 +4796,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B293" t="s">
         <v>29</v>
@@ -3242,7 +4807,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B294" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C294">
         <v>75</v>
@@ -3250,7 +4815,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B296" t="s">
         <v>12</v>
@@ -3261,7 +4826,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B297" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C297">
         <v>43.1</v>
@@ -3269,7 +4834,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B299" t="s">
         <v>12</v>
@@ -3288,7 +4853,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B301" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C301">
         <v>18.600000000000001</v>
@@ -3296,7 +4861,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B302" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C302">
         <v>6.7</v>
@@ -3336,7 +4901,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B308" t="s">
         <v>12</v>
@@ -3355,7 +4920,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B310" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C310">
         <v>18.600000000000001</v>
@@ -3363,7 +4928,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B311" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C311">
         <v>6.7</v>
@@ -3403,7 +4968,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B316" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C316">
         <v>7.2</v>
@@ -3411,7 +4976,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B318" t="s">
         <v>12</v>
@@ -3438,7 +5003,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B321" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C321">
         <v>15.1</v>
@@ -3446,7 +5011,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B322" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C322">
         <v>17.7</v>
@@ -3454,7 +5019,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B323" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C323">
         <v>18.7</v>
@@ -3462,7 +5027,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B325" t="s">
         <v>12</v>
@@ -3489,7 +5054,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B328" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C328">
         <v>15.1</v>
@@ -3497,7 +5062,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B329" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C329">
         <v>17.7</v>
@@ -3505,7 +5070,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B330" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C330">
         <v>13.6</v>
@@ -3513,10 +5078,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B332" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C332">
         <v>0</v>
@@ -3524,7 +5089,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B333" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C333">
         <v>18.7</v>
@@ -3532,7 +5097,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B334" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C334">
         <v>17.7</v>
@@ -3572,10 +5137,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B340" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C340">
         <v>0</v>
@@ -3583,7 +5148,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B341" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C341">
         <v>18.7</v>
@@ -3591,7 +5156,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B342" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C342">
         <v>17.7</v>
@@ -3631,7 +5196,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B347" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C347">
         <v>7.2</v>
@@ -3639,10 +5204,10 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B349" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C349">
         <v>0</v>
@@ -3650,7 +5215,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B350" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C350">
         <v>13.6</v>
@@ -3658,7 +5223,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B351" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C351">
         <v>17.7</v>
@@ -3698,15 +5263,15 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B357" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B358" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C358">
         <v>0</v>
@@ -3714,7 +5279,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B359" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C359">
         <v>13.6</v>
@@ -3754,7 +5319,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B364" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C364">
         <v>7.2</v>
@@ -3762,6 +5327,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate data  found!" error="Station codes must be unique." sqref="E114:E1048576 E2:E111" xr:uid="{A6CFE5FB-E603-4683-AAF7-347654812BBA}">
+      <formula1>COUNTIF($E:$E, E2)=1</formula1>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate data found!" error="Line codes must be unique." sqref="H2:H1048576" xr:uid="{0757F312-BBBD-45A5-9F9B-A47BDF518B53}">
+      <formula1>COUNTIF($H:$H, H2) = 1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>